<commit_message>
nova sgrt : hyperarc 1 loc --> sgrt
</commit_message>
<xml_diff>
--- a/Plancheck/plancheck_data/check_protocol/v19/poumon.xlsx
+++ b/Plancheck/plancheck_data/check_protocol/v19/poumon.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="153">
   <si>
     <t>Name_of check_protocol</t>
   </si>
@@ -455,6 +455,33 @@
   </si>
   <si>
     <t>Poumon</t>
+  </si>
+  <si>
+    <t>AutomaticHighDensityMaterial__</t>
+  </si>
+  <si>
+    <t>Bone</t>
+  </si>
+  <si>
+    <t>DoseReportingMode</t>
+  </si>
+  <si>
+    <t>Dose to medium</t>
+  </si>
+  <si>
+    <t>MaximumAutomaticHighDensityVolumeInCM3__</t>
+  </si>
+  <si>
+    <t>0,50</t>
+  </si>
+  <si>
+    <t>PlanDoseCalculation</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -1441,7 +1468,7 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A32" sqref="A32:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1924,10 +1951,10 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="B32" s="26">
-        <v>0.125</v>
+        <v>144</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>145</v>
       </c>
       <c r="C32" s="26"/>
       <c r="D32" s="26"/>
@@ -1941,7 +1968,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B33" s="26">
         <v>0.125</v>
@@ -1958,10 +1985,10 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="B34" s="26" t="s">
-        <v>5</v>
+        <v>91</v>
+      </c>
+      <c r="B34" s="26">
+        <v>0.125</v>
       </c>
       <c r="C34" s="26"/>
       <c r="D34" s="26"/>
@@ -1975,10 +2002,10 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
-        <v>93</v>
+        <v>146</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>6</v>
+        <v>147</v>
       </c>
       <c r="C35" s="26"/>
       <c r="D35" s="26"/>
@@ -1991,8 +2018,12 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="27"/>
-      <c r="B36" s="26"/>
+      <c r="A36" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>5</v>
+      </c>
       <c r="C36" s="26"/>
       <c r="D36" s="26"/>
       <c r="E36" s="26"/>
@@ -2004,8 +2035,12 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="27"/>
-      <c r="B37" s="26"/>
+      <c r="A37" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>6</v>
+      </c>
       <c r="C37" s="26"/>
       <c r="D37" s="26"/>
       <c r="E37" s="26"/>
@@ -2017,8 +2052,12 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="27"/>
-      <c r="B38" s="26"/>
+      <c r="A38" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>149</v>
+      </c>
       <c r="C38" s="26"/>
       <c r="D38" s="26"/>
       <c r="E38" s="26"/>
@@ -2030,8 +2069,12 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="27"/>
-      <c r="B39" s="26"/>
+      <c r="A39" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>151</v>
+      </c>
       <c r="C39" s="26"/>
       <c r="D39" s="26"/>
       <c r="E39" s="26"/>
@@ -2043,8 +2086,12 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="27"/>
-      <c r="B40" s="26"/>
+      <c r="A40" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>152</v>
+      </c>
       <c r="C40" s="26"/>
       <c r="D40" s="26"/>
       <c r="E40" s="26"/>

</xml_diff>